<commit_message>
Feat: Update disparity analysis to use median
</commit_message>
<xml_diff>
--- a/output/tables/publication_summary_tables.xlsx
+++ b/output/tables/publication_summary_tables.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -35,388 +35,391 @@
     <t xml:space="preserve">community</t>
   </si>
   <si>
+    <t xml:space="preserve">degree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">betweenness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVC_pct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">betweenness_pct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">degree_pct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0001-5139-444X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Americas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States of America</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern America</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0001-6159-4947</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Europe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Italy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Europe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0001-6348-8734</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Kingdom of Great Britain and Northern Ireland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northern Europe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0001-6556-8041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oceania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Australia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Australia and New Zealand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0001-6762-828X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0001-6796-2958</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0001-7015-2075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Netherlands (Kingdom of the)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Europe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0001-7037-089X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southern Asia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0001-7176-4604</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Austria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0001-7687-9267</t>
+  </si>
+  <si>
+    <t xml:space="preserve">China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern Asia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0001-8008-6198</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mexico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central America</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0001-8743-7800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0001-8994-5251</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0001-9123-0845</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ireland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0001-9136-0949</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0001-9139-2721</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0001-9376-8366</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0001-9764-685X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-0139-3913</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-0544-6744</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-0724-5962</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-1241-5225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Germany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-1579-7134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greece</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-2085-0446</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-2198-6740</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portugal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-2294-6521</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-2580-5361</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-2759-6727</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-3332-4621</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-3654-1437</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyprus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Asia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-3745-9128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-4050-3281</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-4300-1551</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thailand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South-eastern Asia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-4617-6197</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-4776-3748</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-4928-2446</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-5094-6326</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-5600-0726</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-6079-3554</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-6365-4082</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-7613-1985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-7723-0635</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-7927-3348</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Republic of Korea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-7993-5540</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-8229-2929</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-8256-6942</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-8270-4022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-8279-9666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0002-9270-8860</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0003-0132-8051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nigeria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0003-0173-0112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0003-0200-2133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0003-0291-2735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0003-0956-7997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0003-1861-8813</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0003-2400-2839</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0003-2463-6735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0003-2516-2412</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Japan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0003-2561-6090</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0003-2734-851X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ghana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0003-3163-6119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brazil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South America</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0003-3345-4538</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0003-3572-268X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0003-4065-5194</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0003-4138-6897</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Türkiye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0003-4144-0208</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0003-4244-2854</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000-0003-4346-3163</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0009-0003-8058-6282</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Romania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern Europe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journal</t>
+  </si>
+  <si>
     <t xml:space="preserve">eigenvector</t>
   </si>
   <si>
-    <t xml:space="preserve">degree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">betweenness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eigenvector_pct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">betweenness_pct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">degree_pct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0001-5139-444X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Americas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United States of America</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northern America</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0001-6159-4947</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Europe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Italy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southern Europe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0001-6348-8734</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United Kingdom of Great Britain and Northern Ireland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northern Europe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0001-6556-8041</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oceania</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Australia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Australia and New Zealand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0001-6762-828X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0001-6796-2958</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0001-7015-2075</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Netherlands (Kingdom of the)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Western Europe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0001-7037-089X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">India</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southern Asia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0001-7176-4604</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Austria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0001-7687-9267</t>
-  </si>
-  <si>
-    <t xml:space="preserve">China</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eastern Asia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0001-8008-6198</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mexico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central America</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0001-8743-7800</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0001-8994-5251</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0001-9123-0845</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ireland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0001-9136-0949</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0001-9139-2721</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0001-9376-8366</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0001-9764-685X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-0139-3913</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-0544-6744</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-0724-5962</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-1241-5225</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Germany</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-1579-7134</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Greece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-2085-0446</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-2198-6740</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portugal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-2294-6521</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-2580-5361</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-2759-6727</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-3332-4621</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-3654-1437</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyprus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Western Asia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-3745-9128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-4050-3281</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sweden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-4300-1551</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thailand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South-eastern Asia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-4617-6197</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-4776-3748</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-4928-2446</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-5094-6326</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-5600-0726</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-6079-3554</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-6365-4082</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-7613-1985</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Denmark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-7723-0635</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-7927-3348</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Republic of Korea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-7993-5540</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-8229-2929</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-8256-6942</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-8270-4022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-8279-9666</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0002-9270-8860</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0003-0132-8051</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Africa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nigeria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Western Africa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0003-0173-0112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0003-0200-2133</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0003-0291-2735</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0003-0956-7997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0003-1861-8813</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0003-2400-2839</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0003-2463-6735</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0003-2516-2412</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Japan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0003-2561-6090</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0003-2734-851X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ghana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0003-3163-6119</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brazil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South America</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0003-3345-4538</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0003-3572-268X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0003-4065-5194</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0003-4138-6897</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Türkiye</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0003-4144-0208</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0003-4244-2854</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0000-0003-4346-3163</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0009-0003-8058-6282</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Romania</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eastern Europe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Journal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean_symbolic_capital</t>
+    <t xml:space="preserve">median_evc</t>
   </si>
   <si>
     <t xml:space="preserve">n_editors</t>
   </si>
   <si>
-    <t xml:space="preserve">gini_symbolic_capital</t>
+    <t xml:space="preserve">gini_evc</t>
   </si>
   <si>
     <t xml:space="preserve">Earth Systems Governance</t>
   </si>
   <si>
-    <t xml:space="preserve">25, FALSE, 23, 14, 18, 3, 4, 5, 24, 14, 18, 14, 14, 14, 14, 14, 21, 1, 9, 19, 18, 20, 13, 3, 4, 9, 17, 5, 19, 20, 13, 13, 13, 21, 7, 11, 14, 18, 19, 13, 21, 12, 12, 12, 16, 12, 17, 15, 20, 9, 9, 5, 16, 16, 11, 9, 22, 2, 2, 2, 2, 2, 23, 0, 14, 3, 13, 4, 9, 5, 0, 0, 0, 18, 8, 18, 3, 1, 3, 3, 3, 3, 11, 19, 8, 4, 9, 4, 6, 10, 12, 12, 12, 12, 12, 11, 8, 7, 12, 9, 12, 12, 12, 8, 4, 4, 7, 9, 9, 5, 1, 0, 1, Earth Systems Governance, Global Environmental Change, Annual Review of Environment and Resources, Ecology and Society, PNAS (Sustainability Science), World Development, International Journal of Precision Engineering and Manufacturing-Green Technology, Renewable Energy, Journal of Industrial Ecology, Sustainability Science, International Journal of Sustainable Development and World Ecology, International Journal of Sustainability in Higher Education, Journal of Cleaner Production, Environmental Innovation and Societal Transitions, Current Opinion in Environmental Sustainability, Sustainable Development, Renewable and Sustainable Energy Reviews, Sustainable Cities and Society, Ecological Economics, Environment, Development, and Sustainability, Sustainable Production and Consumption, Environmental Research Letters, ACS Sustainable Chemistry and Engineering, ChemSusChem, Green Chemistry, 0.150285401538065, 0.0516226304983961, 0.130300817477314, 0.533232309324391, 0.390921191782991, 0.221123380975133, 0.00842058579872462, 0.111494115539966, 0.773018544566316, 0.730332926834188, 0.0230745172118209, 0.305521842486701, 1, 0.286140935103751, 0.361189928505247, 0.151049869456226, 0.15594503875323, 0.115797270084758, 0.218802041962625, 0.291903466669367, 0.34067073911717, 0.11639952736311, 0.00000000000000000195066237697104, 0.000000000000000005529569956968, 0.00000000000000000824279896730325, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 2, 2, 1, 1, 1, 2, 1, 1, 1, 1, 1, 2, 7, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 3, 1, 1, 3, 9, 1, 1, 2, 1, 2, 4, 1, 3, 3, 3, 1, 1, 1, &lt;environment&gt;</t>
+    <t xml:space="preserve">25, FALSE, 23, 14, 18, 3, 4, 5, 24, 14, 18, 14, 14, 14, 14, 14, 21, 1, 9, 19, 18, 20, 13, 3, 4, 9, 17, 5, 19, 20, 13, 13, 13, 21, 7, 11, 14, 18, 19, 13, 21, 12, 12, 12, 16, 12, 17, 15, 20, 9, 9, 5, 16, 16, 11, 9, 22, 2, 2, 2, 2, 2, 23, 0, 14, 3, 13, 4, 9, 5, 0, 0, 0, 18, 8, 18, 3, 1, 3, 3, 3, 3, 11, 19, 8, 4, 9, 4, 6, 10, 12, 12, 12, 12, 12, 11, 8, 7, 12, 9, 12, 12, 12, 8, 4, 4, 7, 9, 9, 5, 1, 0, 1, Earth Systems Governance, Global Environmental Change, Annual Review of Environment and Resources, Ecology and Society, PNAS (Sustainability Science), World Development, International Journal of Precision Engineering and Manufacturing-Green Technology, Renewable Energy, Journal of Industrial Ecology, Sustainability Science, International Journal of Sustainable Development and World Ecology, International Journal of Sustainability in Higher Education, Journal of Cleaner Production, Environmental Innovation and Societal Transitions, Current Opinion in Environmental Sustainability, Sustainable Development, Renewable and Sustainable Energy Reviews, Sustainable Cities and Society, Ecological Economics, Environment, Development, and Sustainability, Sustainable Production and Consumption, Environmental Research Letters, ACS Sustainable Chemistry and Engineering, ChemSusChem, Green Chemistry, 0.150285401538065, 0.0516226304983962, 0.130300817477314, 0.533232309324392, 0.390921191782991, 0.221123380975133, 0.00842058579872464, 0.111494115539966, 0.773018544566316, 0.730332926834188, 0.0230745172118209, 0.305521842486702, 1, 0.286140935103751, 0.361189928505247, 0.151049869456226, 0.15594503875323, 0.115797270084758, 0.218802041962625, 0.291903466669367, 0.34067073911717, 0.11639952736311, 0.0000000000000000160946959671504, 0.0000000000000000250469666155453, 0.0000000000000000161054688560173, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 2, 2, 1, 1, 1, 2, 1, 1, 1, 1, 1, 2, 7, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 3, 1, 1, 3, 9, 1, 1, 2, 1, 2, 4, 1, 3, 3, 3, 1, 1, 1, &lt;environment&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Global Environmental Change</t>
@@ -494,7 +497,7 @@
     <t xml:space="preserve">n</t>
   </si>
   <si>
-    <t xml:space="preserve">mean_sc</t>
+    <t xml:space="preserve">median_sc</t>
   </si>
   <si>
     <t xml:space="preserve">p_value</t>
@@ -887,13 +890,13 @@
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0.825078381085948</v>
+        <v>33</v>
       </c>
       <c r="H2" t="n">
-        <v>33</v>
+        <v>59.9437183909368</v>
       </c>
       <c r="I2" t="n">
-        <v>59.9437183909368</v>
+        <v>0.825078381085947</v>
       </c>
       <c r="J2" t="n">
         <v>0.840579710144927</v>
@@ -925,13 +928,13 @@
         <v>1</v>
       </c>
       <c r="G3" t="n">
+        <v>31</v>
+      </c>
+      <c r="H3" t="n">
+        <v>23.3465964031695</v>
+      </c>
+      <c r="I3" t="n">
         <v>0.791230714825685</v>
-      </c>
-      <c r="H3" t="n">
-        <v>31</v>
-      </c>
-      <c r="I3" t="n">
-        <v>23.3465964031695</v>
       </c>
       <c r="J3" t="n">
         <v>0.710144927536232</v>
@@ -963,13 +966,13 @@
         <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0458282378778819</v>
+        <v>6</v>
       </c>
       <c r="H4" t="n">
-        <v>6</v>
+        <v>8.74660446364781</v>
       </c>
       <c r="I4" t="n">
-        <v>8.74660446364781</v>
+        <v>0.0458282378778817</v>
       </c>
       <c r="J4" t="n">
         <v>0.072463768115942</v>
@@ -1001,13 +1004,13 @@
         <v>1</v>
       </c>
       <c r="G5" t="n">
+        <v>36</v>
+      </c>
+      <c r="H5" t="n">
+        <v>169.688907867048</v>
+      </c>
+      <c r="I5" t="n">
         <v>0.755824440827668</v>
-      </c>
-      <c r="H5" t="n">
-        <v>36</v>
-      </c>
-      <c r="I5" t="n">
-        <v>169.688907867048</v>
       </c>
       <c r="J5" t="n">
         <v>0.695652173913043</v>
@@ -1039,13 +1042,13 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
+        <v>32</v>
+      </c>
+      <c r="H6" t="n">
+        <v>109.73476508946</v>
+      </c>
+      <c r="I6" t="n">
         <v>0.736540948811159</v>
-      </c>
-      <c r="H6" t="n">
-        <v>32</v>
-      </c>
-      <c r="I6" t="n">
-        <v>109.73476508946</v>
       </c>
       <c r="J6" t="n">
         <v>0.623188405797101</v>
@@ -1077,13 +1080,13 @@
         <v>3</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0839331010108217</v>
+        <v>18</v>
       </c>
       <c r="H7" t="n">
-        <v>18</v>
+        <v>25.8395285184372</v>
       </c>
       <c r="I7" t="n">
-        <v>25.8395285184372</v>
+        <v>0.0839331010108214</v>
       </c>
       <c r="J7" t="n">
         <v>0.217391304347826</v>
@@ -1115,13 +1118,13 @@
         <v>3</v>
       </c>
       <c r="G8" t="n">
+        <v>22</v>
+      </c>
+      <c r="H8" t="n">
+        <v>66.8848266701753</v>
+      </c>
+      <c r="I8" t="n">
         <v>0.224289641461437</v>
-      </c>
-      <c r="H8" t="n">
-        <v>22</v>
-      </c>
-      <c r="I8" t="n">
-        <v>66.8848266701753</v>
       </c>
       <c r="J8" t="n">
         <v>0.521739130434783</v>
@@ -1153,13 +1156,13 @@
         <v>2</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0869317804477026</v>
+        <v>12</v>
       </c>
       <c r="H9" t="n">
-        <v>12</v>
+        <v>27.5320447050768</v>
       </c>
       <c r="I9" t="n">
-        <v>27.5320447050768</v>
+        <v>0.0869317804477024</v>
       </c>
       <c r="J9" t="n">
         <v>0.260869565217391</v>
@@ -1191,13 +1194,13 @@
         <v>2</v>
       </c>
       <c r="G10" t="n">
+        <v>11</v>
+      </c>
+      <c r="H10" t="n">
+        <v>8.65528470067944</v>
+      </c>
+      <c r="I10" t="n">
         <v>0.0869113264453915</v>
-      </c>
-      <c r="H10" t="n">
-        <v>11</v>
-      </c>
-      <c r="I10" t="n">
-        <v>8.65528470067944</v>
       </c>
       <c r="J10" t="n">
         <v>0.246376811594203</v>
@@ -1229,13 +1232,13 @@
         <v>1</v>
       </c>
       <c r="G11" t="n">
+        <v>29</v>
+      </c>
+      <c r="H11" t="n">
+        <v>8.92315332577904</v>
+      </c>
+      <c r="I11" t="n">
         <v>0.808209706589134</v>
-      </c>
-      <c r="H11" t="n">
-        <v>29</v>
-      </c>
-      <c r="I11" t="n">
-        <v>8.92315332577904</v>
       </c>
       <c r="J11" t="n">
         <v>0.811594202898551</v>
@@ -1267,16 +1270,16 @@
         <v>3</v>
       </c>
       <c r="G12" t="n">
+        <v>21</v>
+      </c>
+      <c r="H12" t="n">
+        <v>12.8270145579955</v>
+      </c>
+      <c r="I12" t="n">
         <v>0.190997599320272</v>
       </c>
-      <c r="H12" t="n">
-        <v>21</v>
-      </c>
-      <c r="I12" t="n">
-        <v>12.8270145579955</v>
-      </c>
       <c r="J12" t="n">
-        <v>0.478260869565217</v>
+        <v>0.434782608695652</v>
       </c>
       <c r="K12" t="n">
         <v>0.528985507246377</v>
@@ -1305,16 +1308,16 @@
         <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="H13" t="n">
-        <v>31</v>
+        <v>7.45779261588085</v>
       </c>
       <c r="I13" t="n">
-        <v>7.45779261588085</v>
+        <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>0.956521739130435</v>
+        <v>1</v>
       </c>
       <c r="K13" t="n">
         <v>0.260869565217391</v>
@@ -1343,13 +1346,13 @@
         <v>3</v>
       </c>
       <c r="G14" t="n">
+        <v>21</v>
+      </c>
+      <c r="H14" t="n">
+        <v>25.2393052645335</v>
+      </c>
+      <c r="I14" t="n">
         <v>0.167225455974457</v>
-      </c>
-      <c r="H14" t="n">
-        <v>21</v>
-      </c>
-      <c r="I14" t="n">
-        <v>25.2393052645335</v>
       </c>
       <c r="J14" t="n">
         <v>0.36231884057971</v>
@@ -1381,13 +1384,13 @@
         <v>4</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0583970592156719</v>
+        <v>6</v>
       </c>
       <c r="H15" t="n">
-        <v>6</v>
+        <v>4.14768939612458</v>
       </c>
       <c r="I15" t="n">
-        <v>4.14768939612458</v>
+        <v>0.0583970592156717</v>
       </c>
       <c r="J15" t="n">
         <v>0.173913043478261</v>
@@ -1419,13 +1422,13 @@
         <v>1</v>
       </c>
       <c r="G16" t="n">
+        <v>29</v>
+      </c>
+      <c r="H16" t="n">
+        <v>33.9997313391653</v>
+      </c>
+      <c r="I16" t="n">
         <v>0.732651832360709</v>
-      </c>
-      <c r="H16" t="n">
-        <v>29</v>
-      </c>
-      <c r="I16" t="n">
-        <v>33.9997313391653</v>
       </c>
       <c r="J16" t="n">
         <v>0.594202898550725</v>
@@ -1457,13 +1460,13 @@
         <v>3</v>
       </c>
       <c r="G17" t="n">
+        <v>7</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.376068376068376</v>
+      </c>
+      <c r="I17" t="n">
         <v>0.03492724499792</v>
-      </c>
-      <c r="H17" t="n">
-        <v>7</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0.376068376068376</v>
       </c>
       <c r="J17" t="n">
         <v>0.0434782608695652</v>
@@ -1495,13 +1498,13 @@
         <v>3</v>
       </c>
       <c r="G18" t="n">
+        <v>27</v>
+      </c>
+      <c r="H18" t="n">
+        <v>56.9931603987168</v>
+      </c>
+      <c r="I18" t="n">
         <v>0.207572939006937</v>
-      </c>
-      <c r="H18" t="n">
-        <v>27</v>
-      </c>
-      <c r="I18" t="n">
-        <v>56.9931603987168</v>
       </c>
       <c r="J18" t="n">
         <v>0.507246376811594</v>
@@ -1533,13 +1536,13 @@
         <v>3</v>
       </c>
       <c r="G19" t="n">
+        <v>20</v>
+      </c>
+      <c r="H19" t="n">
+        <v>20.9346071418787</v>
+      </c>
+      <c r="I19" t="n">
         <v>0.152458362422687</v>
-      </c>
-      <c r="H19" t="n">
-        <v>20</v>
-      </c>
-      <c r="I19" t="n">
-        <v>20.9346071418787</v>
       </c>
       <c r="J19" t="n">
         <v>0.304347826086957</v>
@@ -1571,13 +1574,13 @@
         <v>3</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0504696248433611</v>
+        <v>11</v>
       </c>
       <c r="H20" t="n">
-        <v>11</v>
+        <v>7.42100246244983</v>
       </c>
       <c r="I20" t="n">
-        <v>7.42100246244983</v>
+        <v>0.0504696248433612</v>
       </c>
       <c r="J20" t="n">
         <v>0.101449275362319</v>
@@ -1609,16 +1612,16 @@
         <v>1</v>
       </c>
       <c r="G21" t="n">
+        <v>31</v>
+      </c>
+      <c r="H21" t="n">
+        <v>23.3465964031695</v>
+      </c>
+      <c r="I21" t="n">
         <v>0.791230714825685</v>
       </c>
-      <c r="H21" t="n">
-        <v>31</v>
-      </c>
-      <c r="I21" t="n">
-        <v>23.3465964031695</v>
-      </c>
       <c r="J21" t="n">
-        <v>0.739130434782609</v>
+        <v>0.72463768115942</v>
       </c>
       <c r="K21" t="n">
         <v>0.63768115942029</v>
@@ -1647,16 +1650,16 @@
         <v>1</v>
       </c>
       <c r="G22" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="H22" t="n">
-        <v>31</v>
+        <v>7.45779261588085</v>
       </c>
       <c r="I22" t="n">
-        <v>7.45779261588085</v>
+        <v>1</v>
       </c>
       <c r="J22" t="n">
-        <v>0.898550724637681</v>
+        <v>0.956521739130435</v>
       </c>
       <c r="K22" t="n">
         <v>0.260869565217391</v>
@@ -1685,13 +1688,13 @@
         <v>5</v>
       </c>
       <c r="G23" t="n">
+        <v>10</v>
+      </c>
+      <c r="H23" t="n">
+        <v>8.71218819753686</v>
+      </c>
+      <c r="I23" t="n">
         <v>0.163638240440472</v>
-      </c>
-      <c r="H23" t="n">
-        <v>10</v>
-      </c>
-      <c r="I23" t="n">
-        <v>8.71218819753686</v>
       </c>
       <c r="J23" t="n">
         <v>0.347826086956522</v>
@@ -1723,13 +1726,13 @@
         <v>4</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0583970592156718</v>
+        <v>6</v>
       </c>
       <c r="H24" t="n">
-        <v>6</v>
+        <v>4.14768939612458</v>
       </c>
       <c r="I24" t="n">
-        <v>4.14768939612458</v>
+        <v>0.0583970592156717</v>
       </c>
       <c r="J24" t="n">
         <v>0.152173913043478</v>
@@ -1761,16 +1764,16 @@
         <v>3</v>
       </c>
       <c r="G25" t="n">
+        <v>21</v>
+      </c>
+      <c r="H25" t="n">
+        <v>12.8270145579955</v>
+      </c>
+      <c r="I25" t="n">
         <v>0.190997599320272</v>
       </c>
-      <c r="H25" t="n">
-        <v>21</v>
-      </c>
-      <c r="I25" t="n">
-        <v>12.8270145579955</v>
-      </c>
       <c r="J25" t="n">
-        <v>0.442028985507246</v>
+        <v>0.492753623188406</v>
       </c>
       <c r="K25" t="n">
         <v>0.528985507246377</v>
@@ -1799,13 +1802,13 @@
         <v>1</v>
       </c>
       <c r="G26" t="n">
-        <v>0.791415183908864</v>
+        <v>31</v>
       </c>
       <c r="H26" t="n">
-        <v>31</v>
+        <v>23.4408244533244</v>
       </c>
       <c r="I26" t="n">
-        <v>23.4408244533244</v>
+        <v>0.791415183908863</v>
       </c>
       <c r="J26" t="n">
         <v>0.760869565217391</v>
@@ -1837,13 +1840,13 @@
         <v>3</v>
       </c>
       <c r="G27" t="n">
+        <v>18</v>
+      </c>
+      <c r="H27" t="n">
+        <v>25.8199658561104</v>
+      </c>
+      <c r="I27" t="n">
         <v>0.0949399243012892</v>
-      </c>
-      <c r="H27" t="n">
-        <v>18</v>
-      </c>
-      <c r="I27" t="n">
-        <v>25.8199658561104</v>
       </c>
       <c r="J27" t="n">
         <v>0.27536231884058</v>
@@ -1875,16 +1878,16 @@
         <v>3</v>
       </c>
       <c r="G28" t="n">
+        <v>21</v>
+      </c>
+      <c r="H28" t="n">
+        <v>12.8270145579955</v>
+      </c>
+      <c r="I28" t="n">
         <v>0.190997599320272</v>
       </c>
-      <c r="H28" t="n">
-        <v>21</v>
-      </c>
-      <c r="I28" t="n">
-        <v>12.8270145579955</v>
-      </c>
       <c r="J28" t="n">
-        <v>0.442028985507246</v>
+        <v>0.420289855072464</v>
       </c>
       <c r="K28" t="n">
         <v>0.528985507246377</v>
@@ -1913,13 +1916,13 @@
         <v>3</v>
       </c>
       <c r="G29" t="n">
+        <v>28</v>
+      </c>
+      <c r="H29" t="n">
+        <v>81.9846860578362</v>
+      </c>
+      <c r="I29" t="n">
         <v>0.432874457552573</v>
-      </c>
-      <c r="H29" t="n">
-        <v>28</v>
-      </c>
-      <c r="I29" t="n">
-        <v>81.9846860578362</v>
       </c>
       <c r="J29" t="n">
         <v>0.579710144927536</v>
@@ -1951,13 +1954,13 @@
         <v>3</v>
       </c>
       <c r="G30" t="n">
+        <v>8</v>
+      </c>
+      <c r="H30" t="n">
+        <v>11.4440361551012</v>
+      </c>
+      <c r="I30" t="n">
         <v>0.0483528402505417</v>
-      </c>
-      <c r="H30" t="n">
-        <v>8</v>
-      </c>
-      <c r="I30" t="n">
-        <v>11.4440361551012</v>
       </c>
       <c r="J30" t="n">
         <v>0.0869565217391304</v>
@@ -1989,13 +1992,13 @@
         <v>4</v>
       </c>
       <c r="G31" t="n">
-        <v>0.0583970592156718</v>
+        <v>6</v>
       </c>
       <c r="H31" t="n">
-        <v>6</v>
+        <v>4.14768939612458</v>
       </c>
       <c r="I31" t="n">
-        <v>4.14768939612458</v>
+        <v>0.0583970592156717</v>
       </c>
       <c r="J31" t="n">
         <v>0.152173913043478</v>
@@ -2027,16 +2030,16 @@
         <v>1</v>
       </c>
       <c r="G32" t="n">
+        <v>31</v>
+      </c>
+      <c r="H32" t="n">
+        <v>23.3465964031695</v>
+      </c>
+      <c r="I32" t="n">
         <v>0.791230714825685</v>
       </c>
-      <c r="H32" t="n">
-        <v>31</v>
-      </c>
-      <c r="I32" t="n">
-        <v>23.3465964031695</v>
-      </c>
       <c r="J32" t="n">
-        <v>0.72463768115942</v>
+        <v>0.739130434782609</v>
       </c>
       <c r="K32" t="n">
         <v>0.63768115942029</v>
@@ -2065,13 +2068,13 @@
         <v>3</v>
       </c>
       <c r="G33" t="n">
+        <v>27</v>
+      </c>
+      <c r="H33" t="n">
+        <v>51.8090543248515</v>
+      </c>
+      <c r="I33" t="n">
         <v>0.242480237915712</v>
-      </c>
-      <c r="H33" t="n">
-        <v>27</v>
-      </c>
-      <c r="I33" t="n">
-        <v>51.8090543248515</v>
       </c>
       <c r="J33" t="n">
         <v>0.536231884057971</v>
@@ -2103,16 +2106,16 @@
         <v>1</v>
       </c>
       <c r="G34" t="n">
+        <v>29</v>
+      </c>
+      <c r="H34" t="n">
+        <v>8.92315332577904</v>
+      </c>
+      <c r="I34" t="n">
         <v>0.808209706589134</v>
       </c>
-      <c r="H34" t="n">
-        <v>29</v>
-      </c>
-      <c r="I34" t="n">
-        <v>8.92315332577904</v>
-      </c>
       <c r="J34" t="n">
-        <v>0.797101449275362</v>
+        <v>0.826086956521739</v>
       </c>
       <c r="K34" t="n">
         <v>0.420289855072464</v>
@@ -2141,13 +2144,13 @@
         <v>3</v>
       </c>
       <c r="G35" t="n">
+        <v>24</v>
+      </c>
+      <c r="H35" t="n">
+        <v>31.9704330155569</v>
+      </c>
+      <c r="I35" t="n">
         <v>0.188698898380241</v>
-      </c>
-      <c r="H35" t="n">
-        <v>24</v>
-      </c>
-      <c r="I35" t="n">
-        <v>31.9704330155569</v>
       </c>
       <c r="J35" t="n">
         <v>0.405797101449275</v>
@@ -2179,16 +2182,16 @@
         <v>3</v>
       </c>
       <c r="G36" t="n">
+        <v>21</v>
+      </c>
+      <c r="H36" t="n">
+        <v>12.8270145579955</v>
+      </c>
+      <c r="I36" t="n">
         <v>0.190997599320272</v>
       </c>
-      <c r="H36" t="n">
-        <v>21</v>
-      </c>
-      <c r="I36" t="n">
-        <v>12.8270145579955</v>
-      </c>
       <c r="J36" t="n">
-        <v>0.492753623188406</v>
+        <v>0.456521739130435</v>
       </c>
       <c r="K36" t="n">
         <v>0.528985507246377</v>
@@ -2217,13 +2220,13 @@
         <v>3</v>
       </c>
       <c r="G37" t="n">
-        <v>0.0789752608604366</v>
+        <v>14</v>
       </c>
       <c r="H37" t="n">
-        <v>14</v>
+        <v>7.24639414592975</v>
       </c>
       <c r="I37" t="n">
-        <v>7.24639414592975</v>
+        <v>0.0789752608604365</v>
       </c>
       <c r="J37" t="n">
         <v>0.202898550724638</v>
@@ -2255,16 +2258,16 @@
         <v>1</v>
       </c>
       <c r="G38" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="H38" t="n">
-        <v>31</v>
+        <v>7.45779261588085</v>
       </c>
       <c r="I38" t="n">
-        <v>7.45779261588085</v>
+        <v>1</v>
       </c>
       <c r="J38" t="n">
-        <v>0.956521739130435</v>
+        <v>0.898550724637681</v>
       </c>
       <c r="K38" t="n">
         <v>0.260869565217391</v>
@@ -2293,13 +2296,13 @@
         <v>1</v>
       </c>
       <c r="G39" t="n">
-        <v>0.791415183908864</v>
+        <v>31</v>
       </c>
       <c r="H39" t="n">
-        <v>31</v>
+        <v>23.4408244533244</v>
       </c>
       <c r="I39" t="n">
-        <v>23.4408244533244</v>
+        <v>0.791415183908863</v>
       </c>
       <c r="J39" t="n">
         <v>0.760869565217391</v>
@@ -2331,13 +2334,13 @@
         <v>1</v>
       </c>
       <c r="G40" t="n">
+        <v>31</v>
+      </c>
+      <c r="H40" t="n">
+        <v>23.4408244533244</v>
+      </c>
+      <c r="I40" t="n">
         <v>0.791415183908864</v>
-      </c>
-      <c r="H40" t="n">
-        <v>31</v>
-      </c>
-      <c r="I40" t="n">
-        <v>23.4408244533244</v>
       </c>
       <c r="J40" t="n">
         <v>0.782608695652174</v>
@@ -2369,16 +2372,16 @@
         <v>1</v>
       </c>
       <c r="G41" t="n">
+        <v>44</v>
+      </c>
+      <c r="H41" t="n">
+        <v>190.28468912693</v>
+      </c>
+      <c r="I41" t="n">
         <v>0.85188211584665</v>
       </c>
-      <c r="H41" t="n">
-        <v>44</v>
-      </c>
-      <c r="I41" t="n">
-        <v>190.28468912693</v>
-      </c>
       <c r="J41" t="n">
-        <v>0.869565217391304</v>
+        <v>0.855072463768116</v>
       </c>
       <c r="K41" t="n">
         <v>0.992753623188406</v>
@@ -2407,16 +2410,16 @@
         <v>1</v>
       </c>
       <c r="G42" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="H42" t="n">
-        <v>31</v>
+        <v>7.45779261588085</v>
       </c>
       <c r="I42" t="n">
-        <v>7.45779261588085</v>
+        <v>1</v>
       </c>
       <c r="J42" t="n">
-        <v>0.898550724637681</v>
+        <v>0.956521739130435</v>
       </c>
       <c r="K42" t="n">
         <v>0.260869565217391</v>
@@ -2445,16 +2448,16 @@
         <v>1</v>
       </c>
       <c r="G43" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="H43" t="n">
-        <v>31</v>
+        <v>7.45779261588085</v>
       </c>
       <c r="I43" t="n">
-        <v>7.45779261588085</v>
+        <v>1</v>
       </c>
       <c r="J43" t="n">
-        <v>1</v>
+        <v>0.956521739130435</v>
       </c>
       <c r="K43" t="n">
         <v>0.260869565217391</v>
@@ -2483,13 +2486,13 @@
         <v>4</v>
       </c>
       <c r="G44" t="n">
-        <v>0.0278381928086926</v>
+        <v>4</v>
       </c>
       <c r="H44" t="n">
-        <v>4</v>
+        <v>0.6</v>
       </c>
       <c r="I44" t="n">
-        <v>0.6</v>
+        <v>0.0278381928086925</v>
       </c>
       <c r="J44" t="n">
         <v>0.0289855072463768</v>
@@ -2521,13 +2524,13 @@
         <v>1</v>
       </c>
       <c r="G45" t="n">
+        <v>30</v>
+      </c>
+      <c r="H45" t="n">
+        <v>72.9246011859708</v>
+      </c>
+      <c r="I45" t="n">
         <v>0.733009500122735</v>
-      </c>
-      <c r="H45" t="n">
-        <v>30</v>
-      </c>
-      <c r="I45" t="n">
-        <v>72.9246011859708</v>
       </c>
       <c r="J45" t="n">
         <v>0.608695652173913</v>
@@ -2559,16 +2562,16 @@
         <v>1</v>
       </c>
       <c r="G46" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="H46" t="n">
-        <v>31</v>
+        <v>7.45779261588085</v>
       </c>
       <c r="I46" t="n">
-        <v>7.45779261588085</v>
+        <v>1</v>
       </c>
       <c r="J46" t="n">
-        <v>0.956521739130435</v>
+        <v>0.898550724637681</v>
       </c>
       <c r="K46" t="n">
         <v>0.260869565217391</v>
@@ -2597,13 +2600,13 @@
         <v>1</v>
       </c>
       <c r="G47" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="H47" t="n">
-        <v>31</v>
+        <v>7.45779261588085</v>
       </c>
       <c r="I47" t="n">
-        <v>7.45779261588085</v>
+        <v>1</v>
       </c>
       <c r="J47" t="n">
         <v>0.956521739130435</v>
@@ -2635,16 +2638,16 @@
         <v>1</v>
       </c>
       <c r="G48" t="n">
+        <v>28</v>
+      </c>
+      <c r="H48" t="n">
+        <v>2.01637806637807</v>
+      </c>
+      <c r="I48" t="n">
         <v>0.752830819215995</v>
       </c>
-      <c r="H48" t="n">
-        <v>28</v>
-      </c>
-      <c r="I48" t="n">
-        <v>2.01637806637807</v>
-      </c>
       <c r="J48" t="n">
-        <v>0.666666666666667</v>
+        <v>0.681159420289855</v>
       </c>
       <c r="K48" t="n">
         <v>0.0942028985507246</v>
@@ -2673,13 +2676,13 @@
         <v>1</v>
       </c>
       <c r="G49" t="n">
-        <v>0.74086376869859</v>
+        <v>32</v>
       </c>
       <c r="H49" t="n">
-        <v>32</v>
+        <v>65.5881719587602</v>
       </c>
       <c r="I49" t="n">
-        <v>65.5881719587602</v>
+        <v>0.740863768698589</v>
       </c>
       <c r="J49" t="n">
         <v>0.63768115942029</v>
@@ -2711,13 +2714,13 @@
         <v>2</v>
       </c>
       <c r="G50" t="n">
+        <v>10</v>
+      </c>
+      <c r="H50" t="n">
+        <v>7.12872084982665</v>
+      </c>
+      <c r="I50" t="n">
         <v>0.051537680791438</v>
-      </c>
-      <c r="H50" t="n">
-        <v>10</v>
-      </c>
-      <c r="I50" t="n">
-        <v>7.12872084982665</v>
       </c>
       <c r="J50" t="n">
         <v>0.115942028985507</v>
@@ -2749,13 +2752,13 @@
         <v>6</v>
       </c>
       <c r="G51" t="n">
-        <v>0.0354861648513937</v>
+        <v>6</v>
       </c>
       <c r="H51" t="n">
-        <v>6</v>
+        <v>7.93713062300019</v>
       </c>
       <c r="I51" t="n">
-        <v>7.93713062300019</v>
+        <v>0.0354861648513936</v>
       </c>
       <c r="J51" t="n">
         <v>0.0579710144927536</v>
@@ -2787,16 +2790,16 @@
         <v>3</v>
       </c>
       <c r="G52" t="n">
+        <v>21</v>
+      </c>
+      <c r="H52" t="n">
+        <v>12.8270145579955</v>
+      </c>
+      <c r="I52" t="n">
         <v>0.190997599320272</v>
       </c>
-      <c r="H52" t="n">
-        <v>21</v>
-      </c>
-      <c r="I52" t="n">
-        <v>12.8270145579955</v>
-      </c>
       <c r="J52" t="n">
-        <v>0.442028985507246</v>
+        <v>0.456521739130435</v>
       </c>
       <c r="K52" t="n">
         <v>0.528985507246377</v>
@@ -2825,13 +2828,13 @@
         <v>1</v>
       </c>
       <c r="G53" t="n">
+        <v>15</v>
+      </c>
+      <c r="H53" t="n">
+        <v>18.0601513424656</v>
+      </c>
+      <c r="I53" t="n">
         <v>0.331107339620035</v>
-      </c>
-      <c r="H53" t="n">
-        <v>15</v>
-      </c>
-      <c r="I53" t="n">
-        <v>18.0601513424656</v>
       </c>
       <c r="J53" t="n">
         <v>0.565217391304348</v>
@@ -2860,16 +2863,16 @@
         <v>16</v>
       </c>
       <c r="F54" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G54" t="n">
+        <v>9</v>
+      </c>
+      <c r="H54" t="n">
+        <v>10.2050395432081</v>
+      </c>
+      <c r="I54" t="n">
         <v>0.12233805444572</v>
-      </c>
-      <c r="H54" t="n">
-        <v>9</v>
-      </c>
-      <c r="I54" t="n">
-        <v>10.2050395432081</v>
       </c>
       <c r="J54" t="n">
         <v>0.289855072463768</v>
@@ -2901,16 +2904,16 @@
         <v>1</v>
       </c>
       <c r="G55" t="n">
-        <v>0.752830819215995</v>
+        <v>28</v>
       </c>
       <c r="H55" t="n">
-        <v>28</v>
+        <v>2.01637806637807</v>
       </c>
       <c r="I55" t="n">
-        <v>2.01637806637807</v>
+        <v>0.752830819215994</v>
       </c>
       <c r="J55" t="n">
-        <v>0.681159420289855</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="K55" t="n">
         <v>0.0942028985507246</v>
@@ -2936,16 +2939,16 @@
         <v>20</v>
       </c>
       <c r="F56" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G56" t="n">
+        <v>9</v>
+      </c>
+      <c r="H56" t="n">
+        <v>1.76865079365079</v>
+      </c>
+      <c r="I56" t="n">
         <v>0.180432763120742</v>
-      </c>
-      <c r="H56" t="n">
-        <v>9</v>
-      </c>
-      <c r="I56" t="n">
-        <v>1.76865079365079</v>
       </c>
       <c r="J56" t="n">
         <v>0.391304347826087</v>
@@ -2977,13 +2980,13 @@
         <v>1</v>
       </c>
       <c r="G57" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="H57" t="n">
-        <v>31</v>
+        <v>7.45779261588085</v>
       </c>
       <c r="I57" t="n">
-        <v>7.45779261588085</v>
+        <v>1</v>
       </c>
       <c r="J57" t="n">
         <v>0.898550724637681</v>
@@ -3015,13 +3018,13 @@
         <v>2</v>
       </c>
       <c r="G58" t="n">
-        <v>0.0583011055563262</v>
+        <v>12</v>
       </c>
       <c r="H58" t="n">
-        <v>12</v>
+        <v>22.3503192173959</v>
       </c>
       <c r="I58" t="n">
-        <v>22.3503192173959</v>
+        <v>0.0583011055563261</v>
       </c>
       <c r="J58" t="n">
         <v>0.130434782608696</v>
@@ -3053,16 +3056,16 @@
         <v>3</v>
       </c>
       <c r="G59" t="n">
+        <v>21</v>
+      </c>
+      <c r="H59" t="n">
+        <v>12.8270145579955</v>
+      </c>
+      <c r="I59" t="n">
         <v>0.190997599320272</v>
       </c>
-      <c r="H59" t="n">
-        <v>21</v>
-      </c>
-      <c r="I59" t="n">
-        <v>12.8270145579955</v>
-      </c>
       <c r="J59" t="n">
-        <v>0.442028985507246</v>
+        <v>0.478260869565217</v>
       </c>
       <c r="K59" t="n">
         <v>0.528985507246377</v>
@@ -3091,13 +3094,13 @@
         <v>1</v>
       </c>
       <c r="G60" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="H60" t="n">
-        <v>31</v>
+        <v>7.45779261588085</v>
       </c>
       <c r="I60" t="n">
-        <v>7.45779261588085</v>
+        <v>1</v>
       </c>
       <c r="J60" t="n">
         <v>0.956521739130435</v>
@@ -3129,16 +3132,16 @@
         <v>3</v>
       </c>
       <c r="G61" t="n">
+        <v>20</v>
+      </c>
+      <c r="H61" t="n">
+        <v>33.4607154128607</v>
+      </c>
+      <c r="I61" t="n">
         <v>0.154358780575309</v>
       </c>
-      <c r="H61" t="n">
-        <v>20</v>
-      </c>
-      <c r="I61" t="n">
-        <v>33.4607154128607</v>
-      </c>
       <c r="J61" t="n">
-        <v>0.333333333333333</v>
+        <v>0.318840579710145</v>
       </c>
       <c r="K61" t="n">
         <v>0.804347826086957</v>
@@ -3167,13 +3170,13 @@
         <v>5</v>
       </c>
       <c r="G62" t="n">
+        <v>5</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I62" t="n">
         <v>0.0843382769839535</v>
-      </c>
-      <c r="H62" t="n">
-        <v>5</v>
-      </c>
-      <c r="I62" t="n">
-        <v>0.1</v>
       </c>
       <c r="J62" t="n">
         <v>0.231884057971014</v>
@@ -3205,13 +3208,13 @@
         <v>1</v>
       </c>
       <c r="G63" t="n">
+        <v>14</v>
+      </c>
+      <c r="H63" t="n">
+        <v>9.12108552180533</v>
+      </c>
+      <c r="I63" t="n">
         <v>0.331086885617724</v>
-      </c>
-      <c r="H63" t="n">
-        <v>14</v>
-      </c>
-      <c r="I63" t="n">
-        <v>9.12108552180533</v>
       </c>
       <c r="J63" t="n">
         <v>0.550724637681159</v>
@@ -3243,13 +3246,13 @@
         <v>1</v>
       </c>
       <c r="G64" t="n">
+        <v>31</v>
+      </c>
+      <c r="H64" t="n">
+        <v>29.0632238857722</v>
+      </c>
+      <c r="I64" t="n">
         <v>0.750094543911801</v>
-      </c>
-      <c r="H64" t="n">
-        <v>31</v>
-      </c>
-      <c r="I64" t="n">
-        <v>29.0632238857722</v>
       </c>
       <c r="J64" t="n">
         <v>0.652173913043478</v>
@@ -3281,13 +3284,13 @@
         <v>3</v>
       </c>
       <c r="G65" t="n">
+        <v>11</v>
+      </c>
+      <c r="H65" t="n">
+        <v>8.72759740584718</v>
+      </c>
+      <c r="I65" t="n">
         <v>0.0717673158343309</v>
-      </c>
-      <c r="H65" t="n">
-        <v>11</v>
-      </c>
-      <c r="I65" t="n">
-        <v>8.72759740584718</v>
       </c>
       <c r="J65" t="n">
         <v>0.188405797101449</v>
@@ -3319,13 +3322,13 @@
         <v>3</v>
       </c>
       <c r="G66" t="n">
+        <v>21</v>
+      </c>
+      <c r="H66" t="n">
+        <v>93.8847667675723</v>
+      </c>
+      <c r="I66" t="n">
         <v>0.173738226251163</v>
-      </c>
-      <c r="H66" t="n">
-        <v>21</v>
-      </c>
-      <c r="I66" t="n">
-        <v>93.8847667675723</v>
       </c>
       <c r="J66" t="n">
         <v>0.376811594202899</v>
@@ -3357,16 +3360,16 @@
         <v>1</v>
       </c>
       <c r="G67" t="n">
+        <v>44</v>
+      </c>
+      <c r="H67" t="n">
+        <v>190.28468912693</v>
+      </c>
+      <c r="I67" t="n">
         <v>0.85188211584665</v>
       </c>
-      <c r="H67" t="n">
-        <v>44</v>
-      </c>
-      <c r="I67" t="n">
-        <v>190.28468912693</v>
-      </c>
       <c r="J67" t="n">
-        <v>0.855072463768116</v>
+        <v>0.869565217391304</v>
       </c>
       <c r="K67" t="n">
         <v>0.992753623188406</v>
@@ -3395,13 +3398,13 @@
         <v>6</v>
       </c>
       <c r="G68" t="n">
+        <v>5</v>
+      </c>
+      <c r="H68" t="n">
+        <v>1.90263157894737</v>
+      </c>
+      <c r="I68" t="n">
         <v>0.013830806098398</v>
-      </c>
-      <c r="H68" t="n">
-        <v>5</v>
-      </c>
-      <c r="I68" t="n">
-        <v>1.90263157894737</v>
       </c>
       <c r="J68" t="n">
         <v>0.0144927536231884</v>
@@ -3433,16 +3436,16 @@
         <v>3</v>
       </c>
       <c r="G69" t="n">
+        <v>20</v>
+      </c>
+      <c r="H69" t="n">
+        <v>33.4607154128607</v>
+      </c>
+      <c r="I69" t="n">
         <v>0.154358780575309</v>
       </c>
-      <c r="H69" t="n">
-        <v>20</v>
-      </c>
-      <c r="I69" t="n">
-        <v>33.4607154128607</v>
-      </c>
       <c r="J69" t="n">
-        <v>0.318840579710145</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="K69" t="n">
         <v>0.804347826086957</v>
@@ -3471,16 +3474,16 @@
         <v>1</v>
       </c>
       <c r="G70" t="n">
+        <v>29</v>
+      </c>
+      <c r="H70" t="n">
+        <v>8.92315332577904</v>
+      </c>
+      <c r="I70" t="n">
         <v>0.808209706589134</v>
       </c>
-      <c r="H70" t="n">
-        <v>29</v>
-      </c>
-      <c r="I70" t="n">
-        <v>8.92315332577904</v>
-      </c>
       <c r="J70" t="n">
-        <v>0.826086956521739</v>
+        <v>0.797101449275362</v>
       </c>
       <c r="K70" t="n">
         <v>0.420289855072464</v>
@@ -3508,56 +3511,56 @@
         <v>128</v>
       </c>
       <c r="B1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B2" t="n">
         <v>0.150285401538065</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.083267127531347</v>
+        <v>0.0583011055563261</v>
       </c>
       <c r="F2" t="n">
         <v>5</v>
       </c>
       <c r="G2" t="n">
-        <v>0.384236686466387</v>
+        <v>0.384236686466388</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.0516226304983962</v>
+      </c>
+      <c r="C3" t="s">
         <v>134</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.0516226304983961</v>
-      </c>
-      <c r="C3" t="s">
-        <v>133</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
@@ -3569,24 +3572,24 @@
         <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>0.284903368518238</v>
+        <v>0.284903368518239</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B4" t="n">
         <v>0.130300817477314</v>
       </c>
       <c r="C4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0604330065600472</v>
+        <v>0.051537680791438</v>
       </c>
       <c r="F4" t="n">
         <v>3</v>
@@ -3597,19 +3600,19 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B5" t="n">
-        <v>0.533232309324391</v>
+        <v>0.533232309324392</v>
       </c>
       <c r="C5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>0.153597799984286</v>
+        <v>0.190997599320272</v>
       </c>
       <c r="F5" t="n">
         <v>11</v>
@@ -3620,19 +3623,19 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B6" t="n">
         <v>0.390921191782991</v>
       </c>
       <c r="C6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>0.123352440002404</v>
+        <v>0.0839331010108214</v>
       </c>
       <c r="F6" t="n">
         <v>7</v>
@@ -3643,19 +3646,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B7" t="n">
         <v>0.221123380975133</v>
       </c>
       <c r="C7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0875734923229663</v>
+        <v>0.081454180935629</v>
       </c>
       <c r="F7" t="n">
         <v>4</v>
@@ -3666,19 +3669,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B8" t="n">
-        <v>0.00842058579872462</v>
+        <v>0.00842058579872464</v>
       </c>
       <c r="C8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D8" t="n">
         <v>2</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0278381928086926</v>
+        <v>0.0278381928086925</v>
       </c>
       <c r="F8" t="n">
         <v>1</v>
@@ -3689,42 +3692,42 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B9" t="n">
         <v>0.111494115539966</v>
       </c>
       <c r="C9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D9" t="n">
         <v>2</v>
       </c>
       <c r="E9" t="n">
-        <v>0.187914063853373</v>
+        <v>0.0583970592156717</v>
       </c>
       <c r="F9" t="n">
         <v>5</v>
       </c>
       <c r="G9" t="n">
-        <v>0.60342711255967</v>
+        <v>0.603427112559671</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B10" t="n">
         <v>0.773018544566316</v>
       </c>
       <c r="C10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D10" t="n">
         <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>0.841255723565861</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>12</v>
@@ -3735,19 +3738,19 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B11" t="n">
         <v>0.730332926834188</v>
       </c>
       <c r="C11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D11" t="n">
         <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>0.274878089318375</v>
+        <v>0.190997599320272</v>
       </c>
       <c r="F11" t="n">
         <v>18</v>
@@ -3758,13 +3761,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B12" t="n">
         <v>0.0230745172118209</v>
       </c>
       <c r="C12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D12" t="n">
         <v>4</v>
@@ -3781,19 +3784,19 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B13" t="n">
-        <v>0.305521842486701</v>
+        <v>0.305521842486702</v>
       </c>
       <c r="C13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D13" t="n">
         <v>3</v>
       </c>
       <c r="E13" t="n">
-        <v>0.474418618435409</v>
+        <v>0.50785241268515</v>
       </c>
       <c r="F13" t="n">
         <v>6</v>
@@ -3804,42 +3807,42 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B14" t="n">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D14" t="n">
         <v>3</v>
       </c>
       <c r="E14" t="n">
-        <v>0.848808860283469</v>
+        <v>0.808209706589134</v>
       </c>
       <c r="F14" t="n">
         <v>30</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0649461957055368</v>
+        <v>0.064946195705537</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B15" t="n">
         <v>0.286140935103751</v>
       </c>
       <c r="C15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D15" t="n">
         <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>0.352643248472657</v>
+        <v>0.286783561766718</v>
       </c>
       <c r="F15" t="n">
         <v>4</v>
@@ -3850,19 +3853,19 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B16" t="n">
         <v>0.361189928505247</v>
       </c>
       <c r="C16" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D16" t="n">
         <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>0.178854817401937</v>
+        <v>0.0869317804477024</v>
       </c>
       <c r="F16" t="n">
         <v>9</v>
@@ -3873,19 +3876,19 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B17" t="n">
         <v>0.151049869456226</v>
       </c>
       <c r="C17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D17" t="n">
         <v>3</v>
       </c>
       <c r="E17" t="n">
-        <v>0.752830819215995</v>
+        <v>0.752830819215994</v>
       </c>
       <c r="F17" t="n">
         <v>2</v>
@@ -3896,36 +3899,36 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B18" t="n">
         <v>0.15594503875323</v>
       </c>
       <c r="C18" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D18" t="n">
         <v>2</v>
       </c>
       <c r="E18" t="n">
-        <v>0.217958634519354</v>
+        <v>0.0583970592156717</v>
       </c>
       <c r="F18" t="n">
         <v>5</v>
       </c>
       <c r="G18" t="n">
-        <v>0.543323127075247</v>
+        <v>0.543323127075248</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B19" t="n">
         <v>0.115797270084758</v>
       </c>
       <c r="C19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D19" t="n">
         <v>5</v>
@@ -3942,19 +3945,19 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B20" t="n">
         <v>0.218802041962625</v>
       </c>
       <c r="C20" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D20" t="n">
         <v>3</v>
       </c>
       <c r="E20" t="n">
-        <v>0.282256758695457</v>
+        <v>0.12233805444572</v>
       </c>
       <c r="F20" t="n">
         <v>5</v>
@@ -3965,19 +3968,19 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B21" t="n">
         <v>0.291903466669367</v>
       </c>
       <c r="C21" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D21" t="n">
         <v>3</v>
       </c>
       <c r="E21" t="n">
-        <v>0.473350200413998</v>
+        <v>0.485831738973213</v>
       </c>
       <c r="F21" t="n">
         <v>6</v>
@@ -3988,19 +3991,19 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B22" t="n">
         <v>0.34067073911717</v>
       </c>
       <c r="C22" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D22" t="n">
         <v>3</v>
       </c>
       <c r="E22" t="n">
-        <v>0.686028052794818</v>
+        <v>0.808209706589134</v>
       </c>
       <c r="F22" t="n">
         <v>5</v>
@@ -4011,19 +4014,19 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B23" t="n">
         <v>0.11639952736311</v>
       </c>
       <c r="C23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D23" t="n">
         <v>1</v>
       </c>
       <c r="E23" t="n">
-        <v>0.27228283507489</v>
+        <v>0.0483528402505417</v>
       </c>
       <c r="F23" t="n">
         <v>3</v>
@@ -4034,20 +4037,18 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B24" t="n">
-        <v>0.00000000000000000195066237697104</v>
+        <v>0.0000000000000000160946959671504</v>
       </c>
       <c r="C24" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D24" t="n">
         <v>6</v>
       </c>
-      <c r="E24" t="e">
-        <v>#NUM!</v>
-      </c>
+      <c r="E24"/>
       <c r="F24" t="n">
         <v>1</v>
       </c>
@@ -4057,20 +4058,18 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B25" t="n">
-        <v>0.000000000000000005529569956968</v>
+        <v>0.0000000000000000250469666155453</v>
       </c>
       <c r="C25" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D25" t="n">
         <v>6</v>
       </c>
-      <c r="E25" t="e">
-        <v>#NUM!</v>
-      </c>
+      <c r="E25"/>
       <c r="F25" t="n">
         <v>2</v>
       </c>
@@ -4080,20 +4079,18 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B26" t="n">
-        <v>0.00000000000000000824279896730325</v>
+        <v>0.0000000000000000161054688560173</v>
       </c>
       <c r="C26" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D26" t="n">
         <v>6</v>
       </c>
-      <c r="E26" t="e">
-        <v>#NUM!</v>
-      </c>
+      <c r="E26"/>
       <c r="F26" t="n">
         <v>1</v>
       </c>
@@ -4120,13 +4117,13 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2">
@@ -4137,10 +4134,10 @@
         <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>0.369913884986963</v>
+        <v>0.190997599320272</v>
       </c>
       <c r="D2" t="n">
-        <v>0.781514815861062</v>
+        <v>0.781532330425559</v>
       </c>
     </row>
     <row r="3">
@@ -4151,10 +4148,10 @@
         <v>53</v>
       </c>
       <c r="C3" t="n">
-        <v>0.45735167288703</v>
+        <v>0.224289641461437</v>
       </c>
       <c r="D3" t="n">
-        <v>0.781514815861062</v>
+        <v>0.781532330425559</v>
       </c>
     </row>
   </sheetData>
@@ -4176,10 +4173,10 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2">
@@ -4201,7 +4198,7 @@
         <v>15</v>
       </c>
       <c r="C3" t="n">
-        <v>0.497932859716286</v>
+        <v>0.732651832360709</v>
       </c>
     </row>
     <row r="4">
@@ -4212,7 +4209,7 @@
         <v>35</v>
       </c>
       <c r="C4" t="n">
-        <v>0.483871348485802</v>
+        <v>0.331086885617724</v>
       </c>
     </row>
     <row r="5">
@@ -4223,7 +4220,7 @@
         <v>15</v>
       </c>
       <c r="C5" t="n">
-        <v>0.271149171673577</v>
+        <v>0.167225455974457</v>
       </c>
     </row>
     <row r="6">
@@ -4234,7 +4231,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0949224727133512</v>
+        <v>0.0949224727133511</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalize analysis scripts and correct all plotting errors
</commit_message>
<xml_diff>
--- a/output/tables/publication_summary_tables.xlsx
+++ b/output/tables/publication_summary_tables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t xml:space="preserve">betweenness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">closeness</t>
   </si>
   <si>
     <t xml:space="preserve">EVC_pct</t>
@@ -894,22 +897,25 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" t="n">
         <v>3</v>
@@ -927,30 +933,33 @@
         <v>59.9437183909368</v>
       </c>
       <c r="K2" t="n">
+        <v>0.00917431192660551</v>
+      </c>
+      <c r="L2" t="n">
         <v>0.840579710144927</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>0.869565217391304</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>0.956521739130435</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" t="n">
         <v>2</v>
@@ -968,30 +977,33 @@
         <v>23.3465964031695</v>
       </c>
       <c r="K3" t="n">
+        <v>0.00900900900900901</v>
+      </c>
+      <c r="L3" t="n">
         <v>0.710144927536232</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>0.63768115942029</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>0.804347826086957</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F4" t="n">
         <v>2</v>
@@ -1009,30 +1021,33 @@
         <v>8.74660446364781</v>
       </c>
       <c r="K4" t="n">
+        <v>0.00684931506849315</v>
+      </c>
+      <c r="L4" t="n">
         <v>0.072463768115942</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>0.391304347826087</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>0.0869565217391304</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F5" t="n">
         <v>2</v>
@@ -1050,30 +1065,33 @@
         <v>169.688907867048</v>
       </c>
       <c r="K5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L5" t="n">
         <v>0.695652173913043</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.971014492753623</v>
       </c>
       <c r="M5" t="n">
         <v>0.971014492753623</v>
       </c>
+      <c r="N5" t="n">
+        <v>0.971014492753623</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F6" t="n">
         <v>2</v>
@@ -1091,30 +1109,33 @@
         <v>109.73476508946</v>
       </c>
       <c r="K6" t="n">
+        <v>0.00925925925925926</v>
+      </c>
+      <c r="L6" t="n">
         <v>0.623188405797101</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>0.956521739130435</v>
       </c>
-      <c r="M6" t="n">
+      <c r="N6" t="n">
         <v>0.934782608695652</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F7" t="n">
         <v>4</v>
@@ -1132,30 +1153,33 @@
         <v>25.8395285184372</v>
       </c>
       <c r="K7" t="n">
+        <v>0.0065359477124183</v>
+      </c>
+      <c r="L7" t="n">
         <v>0.217391304347826</v>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
         <v>0.739130434782609</v>
       </c>
-      <c r="M7" t="n">
+      <c r="N7" t="n">
         <v>0.340579710144928</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F8" t="n">
         <v>2</v>
@@ -1173,30 +1197,33 @@
         <v>66.8848266701753</v>
       </c>
       <c r="K8" t="n">
+        <v>0.00862068965517241</v>
+      </c>
+      <c r="L8" t="n">
         <v>0.521739130434783</v>
       </c>
-      <c r="L8" t="n">
+      <c r="M8" t="n">
         <v>0.898550724637681</v>
       </c>
-      <c r="M8" t="n">
+      <c r="N8" t="n">
         <v>0.521739130434783</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F9" t="n">
         <v>2</v>
@@ -1214,30 +1241,33 @@
         <v>27.5320447050768</v>
       </c>
       <c r="K9" t="n">
+        <v>0.00775193798449612</v>
+      </c>
+      <c r="L9" t="n">
         <v>0.260869565217391</v>
       </c>
-      <c r="L9" t="n">
+      <c r="M9" t="n">
         <v>0.753623188405797</v>
       </c>
-      <c r="M9" t="n">
+      <c r="N9" t="n">
         <v>0.268115942028986</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F10" t="n">
         <v>2</v>
@@ -1255,30 +1285,33 @@
         <v>8.65528470067944</v>
       </c>
       <c r="K10" t="n">
+        <v>0.00757575757575758</v>
+      </c>
+      <c r="L10" t="n">
         <v>0.246376811594203</v>
       </c>
-      <c r="L10" t="n">
+      <c r="M10" t="n">
         <v>0.347826086956522</v>
       </c>
-      <c r="M10" t="n">
+      <c r="N10" t="n">
         <v>0.231884057971014</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" t="n">
         <v>3</v>
@@ -1296,30 +1329,33 @@
         <v>8.92315332577904</v>
       </c>
       <c r="K11" t="n">
+        <v>0.00869565217391304</v>
+      </c>
+      <c r="L11" t="n">
         <v>0.804347826086957</v>
       </c>
-      <c r="L11" t="n">
+      <c r="M11" t="n">
         <v>0.420289855072464</v>
       </c>
-      <c r="M11" t="n">
+      <c r="N11" t="n">
         <v>0.644927536231884</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F12" t="n">
         <v>2</v>
@@ -1337,30 +1373,33 @@
         <v>12.8270145579955</v>
       </c>
       <c r="K12" t="n">
+        <v>0.00806451612903226</v>
+      </c>
+      <c r="L12" t="n">
         <v>0.463768115942029</v>
       </c>
-      <c r="L12" t="n">
+      <c r="M12" t="n">
         <v>0.528985507246377</v>
       </c>
-      <c r="M12" t="n">
+      <c r="N12" t="n">
         <v>0.456521739130435</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F13" t="n">
         <v>2</v>
@@ -1378,30 +1417,33 @@
         <v>7.45779261588085</v>
       </c>
       <c r="K13" t="n">
+        <v>0.00854700854700855</v>
+      </c>
+      <c r="L13" t="n">
         <v>0.985507246376812</v>
       </c>
-      <c r="L13" t="n">
+      <c r="M13" t="n">
         <v>0.260869565217391</v>
       </c>
-      <c r="M13" t="n">
+      <c r="N13" t="n">
         <v>0.804347826086957</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F14" t="n">
         <v>2</v>
@@ -1419,30 +1461,33 @@
         <v>25.2393052645335</v>
       </c>
       <c r="K14" t="n">
+        <v>0.00833333333333333</v>
+      </c>
+      <c r="L14" t="n">
         <v>0.36231884057971</v>
       </c>
-      <c r="L14" t="n">
+      <c r="M14" t="n">
         <v>0.710144927536232</v>
       </c>
-      <c r="M14" t="n">
+      <c r="N14" t="n">
         <v>0.456521739130435</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F15" t="n">
         <v>2</v>
@@ -1460,30 +1505,33 @@
         <v>4.14768939612458</v>
       </c>
       <c r="K15" t="n">
+        <v>0.00657894736842105</v>
+      </c>
+      <c r="L15" t="n">
         <v>0.159420289855072</v>
       </c>
-      <c r="L15" t="n">
+      <c r="M15" t="n">
         <v>0.130434782608696</v>
       </c>
-      <c r="M15" t="n">
+      <c r="N15" t="n">
         <v>0.0869565217391304</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F16" t="n">
         <v>2</v>
@@ -1501,30 +1549,33 @@
         <v>33.9997313391653</v>
       </c>
       <c r="K16" t="n">
+        <v>0.00917431192660551</v>
+      </c>
+      <c r="L16" t="n">
         <v>0.594202898550725</v>
       </c>
-      <c r="L16" t="n">
+      <c r="M16" t="n">
         <v>0.826086956521739</v>
       </c>
-      <c r="M16" t="n">
+      <c r="N16" t="n">
         <v>0.644927536231884</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F17" t="n">
         <v>2</v>
@@ -1542,30 +1593,33 @@
         <v>0.376068376068376</v>
       </c>
       <c r="K17" t="n">
+        <v>0.00595238095238095</v>
+      </c>
+      <c r="L17" t="n">
         <v>0.0434782608695652</v>
       </c>
-      <c r="L17" t="n">
+      <c r="M17" t="n">
         <v>0.0289855072463768</v>
       </c>
-      <c r="M17" t="n">
+      <c r="N17" t="n">
         <v>0.130434782608696</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F18" t="n">
         <v>3</v>
@@ -1583,30 +1637,33 @@
         <v>56.9931603987168</v>
       </c>
       <c r="K18" t="n">
+        <v>0.00869565217391304</v>
+      </c>
+      <c r="L18" t="n">
         <v>0.507246376811594</v>
       </c>
-      <c r="L18" t="n">
+      <c r="M18" t="n">
         <v>0.855072463768116</v>
       </c>
-      <c r="M18" t="n">
+      <c r="N18" t="n">
         <v>0.557971014492754</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F19" t="n">
         <v>2</v>
@@ -1624,30 +1681,33 @@
         <v>20.9346071418787</v>
       </c>
       <c r="K19" t="n">
+        <v>0.00840336134453781</v>
+      </c>
+      <c r="L19" t="n">
         <v>0.304347826086957</v>
       </c>
-      <c r="L19" t="n">
+      <c r="M19" t="n">
         <v>0.594202898550725</v>
       </c>
-      <c r="M19" t="n">
+      <c r="N19" t="n">
         <v>0.376811594202899</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F20" t="n">
         <v>2</v>
@@ -1665,30 +1725,33 @@
         <v>7.42100246244983</v>
       </c>
       <c r="K20" t="n">
+        <v>0.00625</v>
+      </c>
+      <c r="L20" t="n">
         <v>0.101449275362319</v>
       </c>
-      <c r="L20" t="n">
+      <c r="M20" t="n">
         <v>0.188405797101449</v>
       </c>
-      <c r="M20" t="n">
+      <c r="N20" t="n">
         <v>0.231884057971014</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F21" t="n">
         <v>2</v>
@@ -1706,30 +1769,33 @@
         <v>23.3465964031695</v>
       </c>
       <c r="K21" t="n">
+        <v>0.00900900900900901</v>
+      </c>
+      <c r="L21" t="n">
         <v>0.731884057971015</v>
       </c>
-      <c r="L21" t="n">
+      <c r="M21" t="n">
         <v>0.63768115942029</v>
       </c>
-      <c r="M21" t="n">
+      <c r="N21" t="n">
         <v>0.804347826086957</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F22" t="n">
         <v>2</v>
@@ -1747,30 +1813,33 @@
         <v>7.45779261588085</v>
       </c>
       <c r="K22" t="n">
+        <v>0.00854700854700855</v>
+      </c>
+      <c r="L22" t="n">
         <v>0.934782608695652</v>
       </c>
-      <c r="L22" t="n">
+      <c r="M22" t="n">
         <v>0.260869565217391</v>
       </c>
-      <c r="M22" t="n">
+      <c r="N22" t="n">
         <v>0.804347826086957</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F23" t="n">
         <v>2</v>
@@ -1788,30 +1857,33 @@
         <v>8.71218819753686</v>
       </c>
       <c r="K23" t="n">
+        <v>0.00699300699300699</v>
+      </c>
+      <c r="L23" t="n">
         <v>0.347826086956522</v>
       </c>
-      <c r="L23" t="n">
+      <c r="M23" t="n">
         <v>0.36231884057971</v>
       </c>
-      <c r="M23" t="n">
+      <c r="N23" t="n">
         <v>0.195652173913043</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F24" t="n">
         <v>2</v>
@@ -1829,30 +1901,33 @@
         <v>4.14768939612458</v>
       </c>
       <c r="K24" t="n">
+        <v>0.00657894736842105</v>
+      </c>
+      <c r="L24" t="n">
         <v>0.144927536231884</v>
       </c>
-      <c r="L24" t="n">
+      <c r="M24" t="n">
         <v>0.130434782608696</v>
       </c>
-      <c r="M24" t="n">
+      <c r="N24" t="n">
         <v>0.0869565217391304</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F25" t="n">
         <v>2</v>
@@ -1870,30 +1945,33 @@
         <v>12.8270145579955</v>
       </c>
       <c r="K25" t="n">
+        <v>0.00806451612903226</v>
+      </c>
+      <c r="L25" t="n">
         <v>0.434782608695652</v>
       </c>
-      <c r="L25" t="n">
+      <c r="M25" t="n">
         <v>0.528985507246377</v>
       </c>
-      <c r="M25" t="n">
+      <c r="N25" t="n">
         <v>0.456521739130435</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E26" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F26" t="n">
         <v>2</v>
@@ -1911,30 +1989,33 @@
         <v>23.4408244533244</v>
       </c>
       <c r="K26" t="n">
+        <v>0.00900900900900901</v>
+      </c>
+      <c r="L26" t="n">
         <v>0.768115942028985</v>
       </c>
-      <c r="L26" t="n">
+      <c r="M26" t="n">
         <v>0.681159420289855</v>
       </c>
-      <c r="M26" t="n">
+      <c r="N26" t="n">
         <v>0.804347826086957</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F27" t="n">
         <v>2</v>
@@ -1952,30 +2033,33 @@
         <v>25.8199658561104</v>
       </c>
       <c r="K27" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="L27" t="n">
         <v>0.27536231884058</v>
       </c>
-      <c r="L27" t="n">
+      <c r="M27" t="n">
         <v>0.72463768115942</v>
       </c>
-      <c r="M27" t="n">
+      <c r="N27" t="n">
         <v>0.340579710144928</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E28" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F28" t="n">
         <v>2</v>
@@ -1993,30 +2077,33 @@
         <v>12.8270145579955</v>
       </c>
       <c r="K28" t="n">
+        <v>0.00806451612903226</v>
+      </c>
+      <c r="L28" t="n">
         <v>0.420289855072464</v>
       </c>
-      <c r="L28" t="n">
+      <c r="M28" t="n">
         <v>0.528985507246377</v>
       </c>
-      <c r="M28" t="n">
+      <c r="N28" t="n">
         <v>0.456521739130435</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D29" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F29" t="n">
         <v>2</v>
@@ -2034,30 +2121,33 @@
         <v>81.9846860578362</v>
       </c>
       <c r="K29" t="n">
+        <v>0.00909090909090909</v>
+      </c>
+      <c r="L29" t="n">
         <v>0.579710144927536</v>
       </c>
-      <c r="L29" t="n">
+      <c r="M29" t="n">
         <v>0.927536231884058</v>
       </c>
-      <c r="M29" t="n">
+      <c r="N29" t="n">
         <v>0.594202898550725</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D30" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F30" t="n">
         <v>2</v>
@@ -2075,30 +2165,33 @@
         <v>11.4440361551012</v>
       </c>
       <c r="K30" t="n">
+        <v>0.0072992700729927</v>
+      </c>
+      <c r="L30" t="n">
         <v>0.0869565217391304</v>
       </c>
-      <c r="L30" t="n">
+      <c r="M30" t="n">
         <v>0.478260869565217</v>
       </c>
-      <c r="M30" t="n">
+      <c r="N30" t="n">
         <v>0.144927536231884</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D31" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E31" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F31" t="n">
         <v>2</v>
@@ -2116,30 +2209,33 @@
         <v>4.14768939612458</v>
       </c>
       <c r="K31" t="n">
+        <v>0.00657894736842105</v>
+      </c>
+      <c r="L31" t="n">
         <v>0.173913043478261</v>
       </c>
-      <c r="L31" t="n">
+      <c r="M31" t="n">
         <v>0.130434782608696</v>
       </c>
-      <c r="M31" t="n">
+      <c r="N31" t="n">
         <v>0.0869565217391304</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D32" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E32" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F32" t="n">
         <v>2</v>
@@ -2157,30 +2253,33 @@
         <v>23.3465964031695</v>
       </c>
       <c r="K32" t="n">
+        <v>0.00900900900900901</v>
+      </c>
+      <c r="L32" t="n">
         <v>0.731884057971015</v>
       </c>
-      <c r="L32" t="n">
+      <c r="M32" t="n">
         <v>0.63768115942029</v>
       </c>
-      <c r="M32" t="n">
+      <c r="N32" t="n">
         <v>0.804347826086957</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E33" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F33" t="n">
         <v>4</v>
@@ -2198,30 +2297,33 @@
         <v>51.8090543248515</v>
       </c>
       <c r="K33" t="n">
+        <v>0.00819672131147541</v>
+      </c>
+      <c r="L33" t="n">
         <v>0.536231884057971</v>
       </c>
-      <c r="L33" t="n">
+      <c r="M33" t="n">
         <v>0.840579710144927</v>
       </c>
-      <c r="M33" t="n">
+      <c r="N33" t="n">
         <v>0.557971014492754</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C34" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D34" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E34" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F34" t="n">
         <v>2</v>
@@ -2239,30 +2341,33 @@
         <v>8.92315332577904</v>
       </c>
       <c r="K34" t="n">
+        <v>0.00869565217391304</v>
+      </c>
+      <c r="L34" t="n">
         <v>0.826086956521739</v>
       </c>
-      <c r="L34" t="n">
+      <c r="M34" t="n">
         <v>0.420289855072464</v>
       </c>
-      <c r="M34" t="n">
+      <c r="N34" t="n">
         <v>0.644927536231884</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E35" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F35" t="n">
         <v>2</v>
@@ -2280,30 +2385,33 @@
         <v>31.9704330155569</v>
       </c>
       <c r="K35" t="n">
+        <v>0.00869565217391304</v>
+      </c>
+      <c r="L35" t="n">
         <v>0.405797101449275</v>
       </c>
-      <c r="L35" t="n">
+      <c r="M35" t="n">
         <v>0.782608695652174</v>
       </c>
-      <c r="M35" t="n">
+      <c r="N35" t="n">
         <v>0.536231884057971</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B36" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E36" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F36" t="n">
         <v>2</v>
@@ -2321,30 +2429,33 @@
         <v>12.8270145579955</v>
       </c>
       <c r="K36" t="n">
+        <v>0.00806451612903226</v>
+      </c>
+      <c r="L36" t="n">
         <v>0.463768115942029</v>
       </c>
-      <c r="L36" t="n">
+      <c r="M36" t="n">
         <v>0.528985507246377</v>
       </c>
-      <c r="M36" t="n">
+      <c r="N36" t="n">
         <v>0.456521739130435</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B37" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C37" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D37" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E37" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F37" t="n">
         <v>3</v>
@@ -2362,30 +2473,33 @@
         <v>7.24639414592975</v>
       </c>
       <c r="K37" t="n">
+        <v>0.00757575757575758</v>
+      </c>
+      <c r="L37" t="n">
         <v>0.202898550724638</v>
       </c>
-      <c r="L37" t="n">
+      <c r="M37" t="n">
         <v>0.173913043478261</v>
       </c>
-      <c r="M37" t="n">
+      <c r="N37" t="n">
         <v>0.297101449275362</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E38" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F38" t="n">
         <v>2</v>
@@ -2403,30 +2517,33 @@
         <v>7.45779261588085</v>
       </c>
       <c r="K38" t="n">
+        <v>0.00854700854700855</v>
+      </c>
+      <c r="L38" t="n">
         <v>0.985507246376812</v>
       </c>
-      <c r="L38" t="n">
+      <c r="M38" t="n">
         <v>0.260869565217391</v>
       </c>
-      <c r="M38" t="n">
+      <c r="N38" t="n">
         <v>0.804347826086957</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D39" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E39" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F39" t="n">
         <v>2</v>
@@ -2444,30 +2561,33 @@
         <v>23.4408244533244</v>
       </c>
       <c r="K39" t="n">
+        <v>0.00900900900900901</v>
+      </c>
+      <c r="L39" t="n">
         <v>0.768115942028985</v>
       </c>
-      <c r="L39" t="n">
+      <c r="M39" t="n">
         <v>0.681159420289855</v>
       </c>
-      <c r="M39" t="n">
+      <c r="N39" t="n">
         <v>0.804347826086957</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D40" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E40" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F40" t="n">
         <v>2</v>
@@ -2485,30 +2605,33 @@
         <v>23.4408244533244</v>
       </c>
       <c r="K40" t="n">
+        <v>0.00900900900900901</v>
+      </c>
+      <c r="L40" t="n">
         <v>0.768115942028985</v>
       </c>
-      <c r="L40" t="n">
+      <c r="M40" t="n">
         <v>0.681159420289855</v>
       </c>
-      <c r="M40" t="n">
+      <c r="N40" t="n">
         <v>0.804347826086957</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D41" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E41" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F41" t="n">
         <v>2</v>
@@ -2526,30 +2649,33 @@
         <v>190.28468912693</v>
       </c>
       <c r="K41" t="n">
+        <v>0.010752688172043</v>
+      </c>
+      <c r="L41" t="n">
         <v>0.855072463768116</v>
-      </c>
-      <c r="L41" t="n">
-        <v>0.992753623188406</v>
       </c>
       <c r="M41" t="n">
         <v>0.992753623188406</v>
       </c>
+      <c r="N41" t="n">
+        <v>0.992753623188406</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C42" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D42" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E42" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F42" t="n">
         <v>2</v>
@@ -2567,30 +2693,33 @@
         <v>7.45779261588085</v>
       </c>
       <c r="K42" t="n">
+        <v>0.00854700854700855</v>
+      </c>
+      <c r="L42" t="n">
         <v>0.934782608695652</v>
       </c>
-      <c r="L42" t="n">
+      <c r="M42" t="n">
         <v>0.260869565217391</v>
       </c>
-      <c r="M42" t="n">
+      <c r="N42" t="n">
         <v>0.804347826086957</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B43" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C43" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D43" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E43" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F43" t="n">
         <v>2</v>
@@ -2608,30 +2737,33 @@
         <v>7.45779261588085</v>
       </c>
       <c r="K43" t="n">
+        <v>0.00854700854700855</v>
+      </c>
+      <c r="L43" t="n">
         <v>0.891304347826087</v>
       </c>
-      <c r="L43" t="n">
+      <c r="M43" t="n">
         <v>0.260869565217391</v>
       </c>
-      <c r="M43" t="n">
+      <c r="N43" t="n">
         <v>0.804347826086957</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C44" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D44" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E44" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F44" t="n">
         <v>2</v>
@@ -2649,30 +2781,33 @@
         <v>0.6</v>
       </c>
       <c r="K44" t="n">
+        <v>0.00584795321637427</v>
+      </c>
+      <c r="L44" t="n">
         <v>0.0289855072463768</v>
       </c>
-      <c r="L44" t="n">
+      <c r="M44" t="n">
         <v>0.0434782608695652</v>
       </c>
-      <c r="M44" t="n">
+      <c r="N44" t="n">
         <v>0.0144927536231884</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B45" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C45" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D45" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E45" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F45" t="n">
         <v>2</v>
@@ -2690,30 +2825,33 @@
         <v>72.9246011859708</v>
       </c>
       <c r="K45" t="n">
+        <v>0.00934579439252336</v>
+      </c>
+      <c r="L45" t="n">
         <v>0.608695652173913</v>
       </c>
-      <c r="L45" t="n">
+      <c r="M45" t="n">
         <v>0.91304347826087</v>
       </c>
-      <c r="M45" t="n">
+      <c r="N45" t="n">
         <v>0.681159420289855</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C46" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D46" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E46" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F46" t="n">
         <v>2</v>
@@ -2731,30 +2869,33 @@
         <v>7.45779261588085</v>
       </c>
       <c r="K46" t="n">
+        <v>0.00854700854700855</v>
+      </c>
+      <c r="L46" t="n">
         <v>0.934782608695652</v>
       </c>
-      <c r="L46" t="n">
+      <c r="M46" t="n">
         <v>0.260869565217391</v>
       </c>
-      <c r="M46" t="n">
+      <c r="N46" t="n">
         <v>0.804347826086957</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B47" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C47" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D47" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E47" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F47" t="n">
         <v>2</v>
@@ -2772,30 +2913,33 @@
         <v>7.45779261588085</v>
       </c>
       <c r="K47" t="n">
+        <v>0.00854700854700855</v>
+      </c>
+      <c r="L47" t="n">
         <v>0.891304347826087</v>
       </c>
-      <c r="L47" t="n">
+      <c r="M47" t="n">
         <v>0.260869565217391</v>
       </c>
-      <c r="M47" t="n">
+      <c r="N47" t="n">
         <v>0.804347826086957</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B48" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C48" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D48" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E48" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F48" t="n">
         <v>2</v>
@@ -2813,30 +2957,33 @@
         <v>2.01637806637807</v>
       </c>
       <c r="K48" t="n">
+        <v>0.00884955752212389</v>
+      </c>
+      <c r="L48" t="n">
         <v>0.666666666666667</v>
       </c>
-      <c r="L48" t="n">
+      <c r="M48" t="n">
         <v>0.0942028985507246</v>
       </c>
-      <c r="M48" t="n">
+      <c r="N48" t="n">
         <v>0.594202898550725</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B49" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C49" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D49" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E49" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F49" t="n">
         <v>2</v>
@@ -2854,30 +3001,33 @@
         <v>65.5881719587602</v>
       </c>
       <c r="K49" t="n">
+        <v>0.00925925925925926</v>
+      </c>
+      <c r="L49" t="n">
         <v>0.63768115942029</v>
       </c>
-      <c r="L49" t="n">
+      <c r="M49" t="n">
         <v>0.884057971014493</v>
       </c>
-      <c r="M49" t="n">
+      <c r="N49" t="n">
         <v>0.934782608695652</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B50" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C50" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D50" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E50" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F50" t="n">
         <v>2</v>
@@ -2895,30 +3045,33 @@
         <v>7.12872084982665</v>
       </c>
       <c r="K50" t="n">
+        <v>0.0075187969924812</v>
+      </c>
+      <c r="L50" t="n">
         <v>0.115942028985507</v>
       </c>
-      <c r="L50" t="n">
+      <c r="M50" t="n">
         <v>0.159420289855072</v>
       </c>
-      <c r="M50" t="n">
+      <c r="N50" t="n">
         <v>0.195652173913043</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C51" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D51" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E51" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F51" t="n">
         <v>2</v>
@@ -2936,30 +3089,33 @@
         <v>7.93713062300019</v>
       </c>
       <c r="K51" t="n">
+        <v>0.00704225352112676</v>
+      </c>
+      <c r="L51" t="n">
         <v>0.0579710144927536</v>
       </c>
-      <c r="L51" t="n">
+      <c r="M51" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="M51" t="n">
+      <c r="N51" t="n">
         <v>0.0869565217391304</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B52" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C52" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E52" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F52" t="n">
         <v>2</v>
@@ -2977,30 +3133,33 @@
         <v>12.8270145579955</v>
       </c>
       <c r="K52" t="n">
+        <v>0.00806451612903226</v>
+      </c>
+      <c r="L52" t="n">
         <v>0.492753623188406</v>
       </c>
-      <c r="L52" t="n">
+      <c r="M52" t="n">
         <v>0.528985507246377</v>
       </c>
-      <c r="M52" t="n">
+      <c r="N52" t="n">
         <v>0.456521739130435</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B53" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C53" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D53" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E53" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F53" t="n">
         <v>2</v>
@@ -3018,30 +3177,33 @@
         <v>18.0601513424656</v>
       </c>
       <c r="K53" t="n">
+        <v>0.00757575757575758</v>
+      </c>
+      <c r="L53" t="n">
         <v>0.565217391304348</v>
       </c>
-      <c r="L53" t="n">
+      <c r="M53" t="n">
         <v>0.579710144927536</v>
       </c>
-      <c r="M53" t="n">
+      <c r="N53" t="n">
         <v>0.318840579710145</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B54" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C54" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D54" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E54" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F54" t="n">
         <v>2</v>
@@ -3059,30 +3221,33 @@
         <v>10.2050395432081</v>
       </c>
       <c r="K54" t="n">
+        <v>0.00671140939597315</v>
+      </c>
+      <c r="L54" t="n">
         <v>0.289855072463768</v>
       </c>
-      <c r="L54" t="n">
+      <c r="M54" t="n">
         <v>0.463768115942029</v>
       </c>
-      <c r="M54" t="n">
+      <c r="N54" t="n">
         <v>0.166666666666667</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B55" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C55" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D55" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E55" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F55" t="n">
         <v>2</v>
@@ -3100,30 +3265,33 @@
         <v>2.01637806637807</v>
       </c>
       <c r="K55" t="n">
+        <v>0.00884955752212389</v>
+      </c>
+      <c r="L55" t="n">
         <v>0.681159420289855</v>
       </c>
-      <c r="L55" t="n">
+      <c r="M55" t="n">
         <v>0.0942028985507246</v>
       </c>
-      <c r="M55" t="n">
+      <c r="N55" t="n">
         <v>0.594202898550725</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B56" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C56" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D56" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E56" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F56" t="n">
         <v>2</v>
@@ -3141,30 +3309,33 @@
         <v>1.76865079365079</v>
       </c>
       <c r="K56" t="n">
+        <v>0.00617283950617284</v>
+      </c>
+      <c r="L56" t="n">
         <v>0.391304347826087</v>
       </c>
-      <c r="L56" t="n">
+      <c r="M56" t="n">
         <v>0.0579710144927536</v>
       </c>
-      <c r="M56" t="n">
+      <c r="N56" t="n">
         <v>0.166666666666667</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B57" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C57" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D57" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E57" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F57" t="n">
         <v>2</v>
@@ -3182,30 +3353,33 @@
         <v>7.45779261588085</v>
       </c>
       <c r="K57" t="n">
+        <v>0.00854700854700855</v>
+      </c>
+      <c r="L57" t="n">
         <v>0.934782608695652</v>
       </c>
-      <c r="L57" t="n">
+      <c r="M57" t="n">
         <v>0.260869565217391</v>
       </c>
-      <c r="M57" t="n">
+      <c r="N57" t="n">
         <v>0.804347826086957</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B58" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C58" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D58" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E58" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F58" t="n">
         <v>2</v>
@@ -3223,30 +3397,33 @@
         <v>22.3503192173959</v>
       </c>
       <c r="K58" t="n">
+        <v>0.00763358778625954</v>
+      </c>
+      <c r="L58" t="n">
         <v>0.130434782608696</v>
       </c>
-      <c r="L58" t="n">
+      <c r="M58" t="n">
         <v>0.608695652173913</v>
       </c>
-      <c r="M58" t="n">
+      <c r="N58" t="n">
         <v>0.268115942028986</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B59" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C59" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D59" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E59" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F59" t="n">
         <v>2</v>
@@ -3264,30 +3441,33 @@
         <v>12.8270145579955</v>
       </c>
       <c r="K59" t="n">
+        <v>0.00806451612903226</v>
+      </c>
+      <c r="L59" t="n">
         <v>0.463768115942029</v>
       </c>
-      <c r="L59" t="n">
+      <c r="M59" t="n">
         <v>0.528985507246377</v>
       </c>
-      <c r="M59" t="n">
+      <c r="N59" t="n">
         <v>0.456521739130435</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B60" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C60" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D60" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E60" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F60" t="n">
         <v>2</v>
@@ -3305,30 +3485,33 @@
         <v>7.45779261588085</v>
       </c>
       <c r="K60" t="n">
+        <v>0.00854700854700855</v>
+      </c>
+      <c r="L60" t="n">
         <v>0.985507246376812</v>
       </c>
-      <c r="L60" t="n">
+      <c r="M60" t="n">
         <v>0.260869565217391</v>
       </c>
-      <c r="M60" t="n">
+      <c r="N60" t="n">
         <v>0.804347826086957</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B61" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C61" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D61" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E61" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F61" t="n">
         <v>2</v>
@@ -3346,30 +3529,33 @@
         <v>33.4607154128607</v>
       </c>
       <c r="K61" t="n">
+        <v>0.00826446280991736</v>
+      </c>
+      <c r="L61" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="L61" t="n">
+      <c r="M61" t="n">
         <v>0.804347826086957</v>
       </c>
-      <c r="M61" t="n">
+      <c r="N61" t="n">
         <v>0.376811594202899</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B62" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C62" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D62" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E62" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F62" t="n">
         <v>2</v>
@@ -3387,30 +3573,33 @@
         <v>0.1</v>
       </c>
       <c r="K62" t="n">
+        <v>0.00662251655629139</v>
+      </c>
+      <c r="L62" t="n">
         <v>0.231884057971014</v>
       </c>
-      <c r="L62" t="n">
+      <c r="M62" t="n">
         <v>0.0144927536231884</v>
       </c>
-      <c r="M62" t="n">
+      <c r="N62" t="n">
         <v>0.036231884057971</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B63" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C63" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D63" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E63" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F63" t="n">
         <v>2</v>
@@ -3428,30 +3617,33 @@
         <v>9.12108552180533</v>
       </c>
       <c r="K63" t="n">
+        <v>0.00757575757575758</v>
+      </c>
+      <c r="L63" t="n">
         <v>0.550724637681159</v>
       </c>
-      <c r="L63" t="n">
+      <c r="M63" t="n">
         <v>0.449275362318841</v>
       </c>
-      <c r="M63" t="n">
+      <c r="N63" t="n">
         <v>0.297101449275362</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B64" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C64" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D64" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E64" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F64" t="n">
         <v>2</v>
@@ -3469,30 +3661,33 @@
         <v>29.0632238857722</v>
       </c>
       <c r="K64" t="n">
+        <v>0.00934579439252336</v>
+      </c>
+      <c r="L64" t="n">
         <v>0.652173913043478</v>
       </c>
-      <c r="L64" t="n">
+      <c r="M64" t="n">
         <v>0.768115942028985</v>
       </c>
-      <c r="M64" t="n">
+      <c r="N64" t="n">
         <v>0.804347826086957</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B65" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C65" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D65" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E65" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F65" t="n">
         <v>2</v>
@@ -3510,30 +3705,33 @@
         <v>8.72759740584718</v>
       </c>
       <c r="K65" t="n">
+        <v>0.00740740740740741</v>
+      </c>
+      <c r="L65" t="n">
         <v>0.188405797101449</v>
       </c>
-      <c r="L65" t="n">
+      <c r="M65" t="n">
         <v>0.376811594202899</v>
       </c>
-      <c r="M65" t="n">
+      <c r="N65" t="n">
         <v>0.231884057971014</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B66" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C66" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D66" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E66" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F66" t="n">
         <v>2</v>
@@ -3551,30 +3749,33 @@
         <v>93.8847667675723</v>
       </c>
       <c r="K66" t="n">
+        <v>0.00847457627118644</v>
+      </c>
+      <c r="L66" t="n">
         <v>0.376811594202899</v>
       </c>
-      <c r="L66" t="n">
+      <c r="M66" t="n">
         <v>0.942028985507246</v>
       </c>
-      <c r="M66" t="n">
+      <c r="N66" t="n">
         <v>0.456521739130435</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B67" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C67" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D67" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E67" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F67" t="n">
         <v>2</v>
@@ -3592,30 +3793,33 @@
         <v>190.28468912693</v>
       </c>
       <c r="K67" t="n">
+        <v>0.010752688172043</v>
+      </c>
+      <c r="L67" t="n">
         <v>0.869565217391304</v>
-      </c>
-      <c r="L67" t="n">
-        <v>0.992753623188406</v>
       </c>
       <c r="M67" t="n">
         <v>0.992753623188406</v>
       </c>
+      <c r="N67" t="n">
+        <v>0.992753623188406</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B68" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C68" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D68" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E68" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F68" t="n">
         <v>2</v>
@@ -3633,30 +3837,33 @@
         <v>1.90263157894737</v>
       </c>
       <c r="K68" t="n">
+        <v>0.00588235294117647</v>
+      </c>
+      <c r="L68" t="n">
         <v>0.0144927536231884</v>
       </c>
-      <c r="L68" t="n">
+      <c r="M68" t="n">
         <v>0.072463768115942</v>
       </c>
-      <c r="M68" t="n">
+      <c r="N68" t="n">
         <v>0.036231884057971</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B69" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C69" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D69" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E69" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F69" t="n">
         <v>2</v>
@@ -3674,30 +3881,33 @@
         <v>33.4607154128607</v>
       </c>
       <c r="K69" t="n">
+        <v>0.00826446280991736</v>
+      </c>
+      <c r="L69" t="n">
         <v>0.318840579710145</v>
       </c>
-      <c r="L69" t="n">
+      <c r="M69" t="n">
         <v>0.804347826086957</v>
       </c>
-      <c r="M69" t="n">
+      <c r="N69" t="n">
         <v>0.376811594202899</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B70" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C70" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D70" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E70" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F70" t="n">
         <v>2</v>
@@ -3715,12 +3925,15 @@
         <v>8.92315332577904</v>
       </c>
       <c r="K70" t="n">
+        <v>0.00869565217391304</v>
+      </c>
+      <c r="L70" t="n">
         <v>0.804347826086957</v>
       </c>
-      <c r="L70" t="n">
+      <c r="M70" t="n">
         <v>0.420289855072464</v>
       </c>
-      <c r="M70" t="n">
+      <c r="N70" t="n">
         <v>0.644927536231884</v>
       </c>
     </row>
@@ -3740,13 +3953,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -3755,18 +3968,18 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
@@ -3792,7 +4005,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B3" t="n">
         <v>3</v>
@@ -3818,7 +4031,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B4" t="n">
         <v>2</v>
@@ -3844,7 +4057,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B5" t="n">
         <v>9</v>
@@ -3870,7 +4083,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B6" t="n">
         <v>5</v>
@@ -3896,7 +4109,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B7" t="n">
         <v>5</v>
@@ -3922,7 +4135,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B8" t="n">
         <v>11</v>
@@ -3948,7 +4161,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B9" t="n">
         <v>6</v>
@@ -3974,7 +4187,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B10" t="n">
         <v>4</v>
@@ -4000,7 +4213,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B11" t="n">
         <v>3</v>
@@ -4026,7 +4239,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B12" t="n">
         <v>2</v>
@@ -4052,7 +4265,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -4078,7 +4291,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B14" t="n">
         <v>1</v>
@@ -4104,7 +4317,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B15" t="n">
         <v>6</v>
@@ -4130,7 +4343,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B16" t="n">
         <v>1</v>
@@ -4156,7 +4369,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B17" t="n">
         <v>29</v>
@@ -4182,7 +4395,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B18" t="n">
         <v>12</v>
@@ -4208,7 +4421,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B19" t="n">
         <v>7</v>
@@ -4234,7 +4447,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B20" t="n">
         <v>5</v>
@@ -4260,7 +4473,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B21" t="n">
         <v>5</v>
@@ -4286,7 +4499,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B22" t="n">
         <v>18</v>
@@ -4312,7 +4525,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B23" t="n">
         <v>2</v>
@@ -4338,7 +4551,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B24" t="n">
         <v>2</v>
@@ -4364,7 +4577,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B25" t="n">
         <v>5</v>
@@ -4390,7 +4603,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B26" t="n">
         <v>4</v>
@@ -4433,18 +4646,18 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" t="n">
         <v>16</v>
@@ -4458,7 +4671,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" t="n">
         <v>53</v>
@@ -4489,18 +4702,18 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B2" t="n">
         <v>2</v>
@@ -4514,7 +4727,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" t="n">
         <v>15</v>
@@ -4528,7 +4741,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B4" t="n">
         <v>15</v>
@@ -4542,7 +4755,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" t="n">
         <v>35</v>
@@ -4556,7 +4769,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" t="n">
         <v>2</v>
@@ -4584,25 +4797,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -4611,18 +4824,18 @@
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
@@ -4658,7 +4871,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B3" t="n">
         <v>3</v>
@@ -4696,7 +4909,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B4" t="n">
         <v>2</v>
@@ -4732,7 +4945,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B5" t="n">
         <v>9</v>
@@ -4770,7 +4983,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B6" t="n">
         <v>5</v>
@@ -4808,7 +5021,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B7" t="n">
         <v>5</v>
@@ -4846,7 +5059,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B8" t="n">
         <v>11</v>
@@ -4884,7 +5097,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B9" t="n">
         <v>6</v>
@@ -4922,7 +5135,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B10" t="n">
         <v>4</v>
@@ -4960,7 +5173,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B11" t="n">
         <v>3</v>
@@ -4998,7 +5211,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B12" t="n">
         <v>2</v>
@@ -5036,7 +5249,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -5072,7 +5285,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B14" t="n">
         <v>1</v>
@@ -5110,7 +5323,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B15" t="n">
         <v>6</v>
@@ -5148,7 +5361,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B16" t="n">
         <v>1</v>
@@ -5186,7 +5399,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B17" t="n">
         <v>30</v>
@@ -5224,7 +5437,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B18" t="n">
         <v>12</v>
@@ -5262,7 +5475,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B19" t="n">
         <v>7</v>
@@ -5300,7 +5513,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B20" t="n">
         <v>5</v>
@@ -5338,7 +5551,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B21" t="n">
         <v>5</v>
@@ -5376,7 +5589,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B22" t="n">
         <v>18</v>
@@ -5414,7 +5627,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B23" t="n">
         <v>2</v>
@@ -5452,7 +5665,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B24" t="n">
         <v>2</v>
@@ -5490,7 +5703,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B25" t="n">
         <v>5</v>
@@ -5528,7 +5741,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B26" t="n">
         <v>4</v>

</xml_diff>

<commit_message>
Add subregion and country geographic disparities
</commit_message>
<xml_diff>
--- a/output/tables/publication_summary_tables.xlsx
+++ b/output/tables/publication_summary_tables.xlsx
@@ -933,7 +933,7 @@
         <v>59.9437183909368</v>
       </c>
       <c r="K2" t="n">
-        <v>0.00917431192660551</v>
+        <v>0.0091743119266055</v>
       </c>
       <c r="L2" t="n">
         <v>0.840579710144927</v>
@@ -1549,7 +1549,7 @@
         <v>33.9997313391653</v>
       </c>
       <c r="K16" t="n">
-        <v>0.00917431192660551</v>
+        <v>0.0091743119266055</v>
       </c>
       <c r="L16" t="n">
         <v>0.594202898550725</v>
@@ -2992,7 +2992,7 @@
         <v>1</v>
       </c>
       <c r="H49" t="n">
-        <v>0.740863768698589</v>
+        <v>0.74086376869859</v>
       </c>
       <c r="I49" t="n">
         <v>32</v>

</xml_diff>